<commit_message>
Update on 20201019 part 2
</commit_message>
<xml_diff>
--- a/文档/其他文档/Others/PC/一体机和笔记本软件列表.xlsx
+++ b/文档/其他文档/Others/PC/一体机和笔记本软件列表.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12,14 +12,14 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$G$53</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$G$55</definedName>
   </definedNames>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="90">
   <si>
     <t>是否绿色版</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -109,10 +109,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>硬件信息查看软件 Aida</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>软碟通 UltraISO</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -350,6 +346,37 @@
   </si>
   <si>
     <t>火绒安全软件（未来启用）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">iPhone手机管理软件 爱思助手 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>√</t>
+  </si>
+  <si>
+    <t>√</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>√</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.i4.cn/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>影音播放器 Ace Stream</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://ace-stream.en.softonic.com/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>硬件信息查看软件 Aida64</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -519,13 +546,20 @@
     <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
     <cellStyle name="超链接" xfId="1" builtinId="8"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -537,9 +571,9 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <colors>
     <mruColors>
+      <color rgb="FFFF6699"/>
       <color rgb="FFFFFF66"/>
       <color rgb="FFCC6600"/>
-      <color rgb="FFFF6699"/>
       <color rgb="FF008080"/>
     </mruColors>
   </colors>
@@ -547,12 +581,15 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -594,7 +631,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -629,7 +666,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -838,29 +875,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G53"/>
+  <dimension ref="A1:G55"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.25" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="111.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="111.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>55</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>56</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
@@ -872,12 +909,12 @@
         <v>0</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B2" s="11" t="s">
         <v>4</v>
@@ -894,9 +931,9 @@
       </c>
       <c r="G2" s="12"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B3" s="11" t="s">
         <v>4</v>
@@ -913,9 +950,9 @@
       </c>
       <c r="G3" s="12"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B4" s="16"/>
       <c r="C4" s="16" t="s">
@@ -927,10 +964,10 @@
       <c r="E4" s="16"/>
       <c r="F4" s="16"/>
       <c r="G4" s="24" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
         <v>5</v>
       </c>
@@ -947,7 +984,7 @@
       <c r="F5" s="11"/>
       <c r="G5" s="12"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
         <v>10</v>
       </c>
@@ -964,7 +1001,7 @@
       <c r="F6" s="11"/>
       <c r="G6" s="12"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
@@ -980,10 +1017,10 @@
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
       <c r="G7" s="25" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -999,12 +1036,12 @@
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
       <c r="G8" s="26" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B9" s="11" t="s">
         <v>4</v>
@@ -1021,7 +1058,7 @@
       </c>
       <c r="G9" s="12"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>18</v>
       </c>
@@ -1037,188 +1074,186 @@
       <c r="E10" s="7"/>
       <c r="F10" s="7"/>
       <c r="G10" s="18" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A11" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="B11" s="7"/>
-      <c r="C11" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="F11" s="7"/>
-      <c r="G11" s="8"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.15">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="C11" s="12"/>
+      <c r="D11" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="19" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="B12" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C12" s="8"/>
-      <c r="D12" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="E12" s="7"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7" t="s">
+        <v>4</v>
+      </c>
       <c r="F12" s="7"/>
-      <c r="G12" s="18" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="G12" s="8"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>17</v>
+        <v>52</v>
       </c>
       <c r="B13" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C13" s="27" t="s">
-        <v>4</v>
-      </c>
+      <c r="C13" s="27"/>
       <c r="D13" s="7" t="s">
         <v>4</v>
       </c>
       <c r="E13" s="7"/>
       <c r="F13" s="7"/>
       <c r="G13" s="18" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="18" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G15" s="6"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D16" s="11"/>
+      <c r="E16" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="F16" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="G16" s="12"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="26" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A14" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="G14" s="6"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A15" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="B15" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="C15" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="D15" s="11"/>
-      <c r="E15" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="F15" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="G15" s="12"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A16" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="26" t="s">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D18" s="11"/>
+      <c r="E18" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="F18" s="11"/>
+      <c r="G18" s="12"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="B19" s="11"/>
+      <c r="C19" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="E19" s="11"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="19" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A17" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="B17" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="C17" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="D17" s="11"/>
-      <c r="E17" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="F17" s="11"/>
-      <c r="G17" s="12"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A18" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="B18" s="11"/>
-      <c r="C18" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="D18" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="E18" s="11"/>
-      <c r="F18" s="11"/>
-      <c r="G18" s="19" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A19" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="B19" s="5"/>
-      <c r="C19" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="20" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A20" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="B20" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="C20" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="D20" s="11"/>
-      <c r="E20" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="F20" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="G20" s="12"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="20" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="11" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B21" s="11" t="s">
         <v>4</v>
@@ -1230,169 +1265,169 @@
       <c r="E21" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="F21" s="11"/>
+      <c r="F21" s="11" t="s">
+        <v>4</v>
+      </c>
       <c r="G21" s="12"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A22" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-      <c r="G22" s="21" t="s">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B22" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D22" s="11"/>
+      <c r="E22" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="F22" s="11"/>
+      <c r="G22" s="12"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="21" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="B24" s="16"/>
+      <c r="C24" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="D24" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="E24" s="16"/>
+      <c r="F24" s="16"/>
+      <c r="G24" s="24" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="B25" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="C25" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D25" s="13"/>
+      <c r="E25" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="F25" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="G25" s="14"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="B26" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="C26" s="16"/>
+      <c r="D26" s="16"/>
+      <c r="E26" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="F26" s="16"/>
+      <c r="G26" s="17"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="B27" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="C27" s="14"/>
+      <c r="D27" s="14"/>
+      <c r="E27" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="F27" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="G27" s="14"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B28" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D28" s="9"/>
+      <c r="E28" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="F28" s="9"/>
+      <c r="G28" s="10"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="B29" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="C29" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="D29" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="E29" s="15"/>
+      <c r="F29" s="15"/>
+      <c r="G29" s="22" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A23" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="B23" s="16"/>
-      <c r="C23" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="D23" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="E23" s="16"/>
-      <c r="F23" s="16"/>
-      <c r="G23" s="24" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A24" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="B24" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="C24" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="D24" s="13"/>
-      <c r="E24" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="F24" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="G24" s="14"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A25" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="B25" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="C25" s="16"/>
-      <c r="D25" s="16"/>
-      <c r="E25" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="F25" s="16"/>
-      <c r="G25" s="17"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A26" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="B26" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="C26" s="14"/>
-      <c r="D26" s="14"/>
-      <c r="E26" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="F26" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="G26" s="14"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A27" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B27" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="C27" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D27" s="9"/>
-      <c r="E27" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="F27" s="9"/>
-      <c r="G27" s="10"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A28" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="B28" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="C28" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="D28" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="E28" s="15"/>
-      <c r="F28" s="15"/>
-      <c r="G28" s="22" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A29" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B29" s="3"/>
-      <c r="C29" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D29" s="3"/>
-      <c r="E29" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F29" s="3"/>
-      <c r="G29" s="4"/>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A30" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="B30" s="11"/>
-      <c r="C30" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="D30" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="E30" s="11"/>
-      <c r="F30" s="11"/>
-      <c r="G30" s="19" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B30" s="3"/>
+      <c r="C30" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F30" s="3"/>
+      <c r="G30" s="4"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="B31" s="11" t="s">
-        <v>4</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="B31" s="11"/>
       <c r="C31" s="11" t="s">
         <v>4</v>
       </c>
@@ -1402,12 +1437,12 @@
       <c r="E31" s="11"/>
       <c r="F31" s="11"/>
       <c r="G31" s="19" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.15">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="11" t="s">
-        <v>51</v>
+        <v>22</v>
       </c>
       <c r="B32" s="11" t="s">
         <v>4</v>
@@ -1415,90 +1450,90 @@
       <c r="C32" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D32" s="11"/>
-      <c r="E32" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="F32" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="G32" s="12"/>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A33" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B33" s="3"/>
-      <c r="C33" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D33" s="3"/>
-      <c r="E33" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F33" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="G33" s="4"/>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="D32" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="E32" s="11"/>
+      <c r="F32" s="11"/>
+      <c r="G32" s="19" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="B33" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C33" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D33" s="11"/>
+      <c r="E33" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="F33" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="G33" s="12"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B34" s="3"/>
       <c r="C34" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D34" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E34" s="3"/>
-      <c r="F34" s="3"/>
-      <c r="G34" s="26" t="s">
+      <c r="D34" s="3"/>
+      <c r="E34" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F34" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G34" s="4"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B35" s="3"/>
+      <c r="C35" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E35" s="3"/>
+      <c r="F35" s="3"/>
+      <c r="G35" s="26" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B36" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C36" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D36" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="E36" s="11"/>
+      <c r="F36" s="11"/>
+      <c r="G36" s="19" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A35" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="B35" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="C35" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="D35" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="E35" s="11"/>
-      <c r="F35" s="11"/>
-      <c r="G35" s="19" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A36" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="B36" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="C36" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="D36" s="13"/>
-      <c r="E36" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="F36" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="G36" s="14"/>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="13" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B37" s="13" t="s">
         <v>4</v>
@@ -1515,26 +1550,28 @@
       </c>
       <c r="G37" s="14"/>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A38" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="B38" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="C38" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="D38" s="11"/>
-      <c r="E38" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="F38" s="11"/>
-      <c r="G38" s="12"/>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B38" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="C38" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D38" s="13"/>
+      <c r="E38" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="F38" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="G38" s="14"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="11" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="B39" s="11" t="s">
         <v>4</v>
@@ -1546,122 +1583,120 @@
       <c r="E39" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="F39" s="11" t="s">
-        <v>4</v>
-      </c>
+      <c r="F39" s="11"/>
       <c r="G39" s="12"/>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A40" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B40" s="3"/>
-      <c r="C40" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D40" s="3"/>
-      <c r="E40" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F40" s="3"/>
-      <c r="G40" s="4"/>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A41" s="9" t="s">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="B40" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C40" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D40" s="11"/>
+      <c r="E40" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="F40" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="G40" s="12"/>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B41" s="3"/>
+      <c r="C41" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D41" s="3"/>
+      <c r="E41" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F41" s="3"/>
+      <c r="G41" s="4"/>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B41" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="C41" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D41" s="9"/>
-      <c r="E41" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="F41" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="G41" s="10"/>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A42" s="9" t="s">
-        <v>40</v>
-      </c>
       <c r="B42" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C42" s="9"/>
-      <c r="D42" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="E42" s="9"/>
-      <c r="F42" s="9"/>
-      <c r="G42" s="23" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A43" s="5" t="s">
+      <c r="C42" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D42" s="9"/>
+      <c r="E42" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="F42" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="G42" s="10"/>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B43" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C43" s="9"/>
+      <c r="D43" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E43" s="9"/>
+      <c r="F43" s="9"/>
+      <c r="G43" s="23" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B43" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C43" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D43" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="E43" s="5"/>
-      <c r="F43" s="5"/>
-      <c r="G43" s="20" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A44" s="11" t="s">
+      <c r="B44" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C44" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D44" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E44" s="5"/>
+      <c r="F44" s="5"/>
+      <c r="G44" s="20" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B44" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="C44" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="D44" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="E44" s="11"/>
-      <c r="F44" s="11"/>
-      <c r="G44" s="19" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A45" s="11" t="s">
-        <v>24</v>
-      </c>
       <c r="B45" s="11" t="s">
         <v>4</v>
       </c>
       <c r="C45" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D45" s="11"/>
-      <c r="E45" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="F45" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="G45" s="12"/>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="D45" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="E45" s="11"/>
+      <c r="F45" s="11"/>
+      <c r="G45" s="19" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="11" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B46" s="11" t="s">
         <v>4</v>
@@ -1678,140 +1713,176 @@
       </c>
       <c r="G46" s="12"/>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B47" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C47" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D47" s="11"/>
+      <c r="E47" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="F47" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="G47" s="12"/>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B47" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="C47" s="11"/>
-      <c r="D47" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="E47" s="11"/>
-      <c r="F47" s="11"/>
-      <c r="G47" s="19" t="s">
+      <c r="B48" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="C48" s="11"/>
+      <c r="D48" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="E48" s="11"/>
+      <c r="F48" s="11"/>
+      <c r="G48" s="19" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B49" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C49" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D49" s="11"/>
+      <c r="E49" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="F49" s="11"/>
+      <c r="G49" s="12"/>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="B50" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="C50" s="10"/>
+      <c r="D50" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="E50" s="10"/>
+      <c r="F50" s="10"/>
+      <c r="G50" s="23" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B51" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C51" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D51" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E51" s="9"/>
+      <c r="F51" s="9"/>
+      <c r="G51" s="23" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A52" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="B52" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C52" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D52" s="11"/>
+      <c r="E52" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="F52" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="G52" s="12"/>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="B53" s="11"/>
+      <c r="C53" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D53" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="E53" s="11"/>
+      <c r="F53" s="11"/>
+      <c r="G53" s="19" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A48" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B48" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="C48" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="D48" s="11"/>
-      <c r="E48" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="F48" s="11"/>
-      <c r="G48" s="12"/>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A49" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B49" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="C49" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D49" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="E49" s="9"/>
-      <c r="F49" s="9"/>
-      <c r="G49" s="23" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A50" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="B50" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="C50" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="D50" s="11"/>
-      <c r="E50" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="F50" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="G50" s="12"/>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A51" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="B51" s="11"/>
-      <c r="C51" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="D51" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="E51" s="11"/>
-      <c r="F51" s="11"/>
-      <c r="G51" s="19" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A52" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="B52" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="C52" s="15"/>
-      <c r="D52" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="E52" s="15"/>
-      <c r="F52" s="15"/>
-      <c r="G52" s="22" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A53" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="B53" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="C53" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="D53" s="13"/>
-      <c r="E53" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="F53" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="G53" s="14"/>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A54" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="B54" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="C54" s="15"/>
+      <c r="D54" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="E54" s="15"/>
+      <c r="F54" s="15"/>
+      <c r="G54" s="22" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A55" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B55" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="C55" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D55" s="13"/>
+      <c r="E55" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="F55" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="G55" s="14"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G53">
-    <sortState ref="A2:G53">
+  <autoFilter ref="A1:G55">
+    <sortState ref="A2:G55">
       <sortCondition ref="A1:A53"/>
     </sortState>
   </autoFilter>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="浏览器">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="浏览器">
       <formula>NOT(ISERROR(SEARCH("浏览器",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1820,28 +1891,30 @@
     <hyperlink ref="G7" r:id="rId2"/>
     <hyperlink ref="G8" r:id="rId3" location="product-desktop-release"/>
     <hyperlink ref="G10" r:id="rId4"/>
-    <hyperlink ref="G12" r:id="rId5"/>
-    <hyperlink ref="G13" r:id="rId6"/>
-    <hyperlink ref="G16" r:id="rId7"/>
-    <hyperlink ref="G18" r:id="rId8"/>
-    <hyperlink ref="G30" r:id="rId9"/>
-    <hyperlink ref="G19" r:id="rId10"/>
-    <hyperlink ref="G22" r:id="rId11"/>
-    <hyperlink ref="G28" r:id="rId12"/>
-    <hyperlink ref="G31" r:id="rId13"/>
-    <hyperlink ref="G34" r:id="rId14"/>
-    <hyperlink ref="G35" r:id="rId15"/>
-    <hyperlink ref="G44" r:id="rId16"/>
-    <hyperlink ref="G47" r:id="rId17"/>
-    <hyperlink ref="G51" r:id="rId18"/>
-    <hyperlink ref="G42" r:id="rId19" location="/download"/>
-    <hyperlink ref="G52" r:id="rId20"/>
-    <hyperlink ref="G43" r:id="rId21"/>
-    <hyperlink ref="G49" r:id="rId22"/>
-    <hyperlink ref="G23" r:id="rId23"/>
+    <hyperlink ref="G13" r:id="rId5"/>
+    <hyperlink ref="G14" r:id="rId6"/>
+    <hyperlink ref="G17" r:id="rId7"/>
+    <hyperlink ref="G19" r:id="rId8"/>
+    <hyperlink ref="G31" r:id="rId9"/>
+    <hyperlink ref="G20" r:id="rId10"/>
+    <hyperlink ref="G23" r:id="rId11"/>
+    <hyperlink ref="G29" r:id="rId12"/>
+    <hyperlink ref="G32" r:id="rId13"/>
+    <hyperlink ref="G35" r:id="rId14"/>
+    <hyperlink ref="G36" r:id="rId15"/>
+    <hyperlink ref="G45" r:id="rId16"/>
+    <hyperlink ref="G48" r:id="rId17"/>
+    <hyperlink ref="G53" r:id="rId18"/>
+    <hyperlink ref="G43" r:id="rId19" location="/download"/>
+    <hyperlink ref="G54" r:id="rId20"/>
+    <hyperlink ref="G44" r:id="rId21"/>
+    <hyperlink ref="G51" r:id="rId22"/>
+    <hyperlink ref="G24" r:id="rId23"/>
+    <hyperlink ref="G11" r:id="rId24"/>
+    <hyperlink ref="G50" r:id="rId25"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId24"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId26"/>
 </worksheet>
 </file>
 
@@ -1851,7 +1924,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1864,7 +1937,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update on 20210121 part 2
</commit_message>
<xml_diff>
--- a/文档/其他文档/Others/PC/一体机和笔记本软件列表.xlsx
+++ b/文档/其他文档/Others/PC/一体机和笔记本软件列表.xlsx
@@ -12,14 +12,14 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$H$61</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$H$62</definedName>
   </definedNames>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="102">
   <si>
     <t>是否绿色版</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -41,10 +41,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Adobe Flash Player去除区域限制版</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Firefox浏览器</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -421,6 +417,14 @@
   </si>
   <si>
     <t>是否为工作需要的软件</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">恢复Win 7样式开始菜单软件 StartIsBack+ </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Adobe Flash Player去除Helper特别版</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -913,14 +917,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:I61"/>
+  <dimension ref="A1:I62"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="35.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="42.5" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="13.875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20.5" bestFit="1" customWidth="1"/>
@@ -931,13 +934,13 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>52</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
@@ -949,22 +952,22 @@
         <v>0</v>
       </c>
       <c r="G1" s="28" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I1" s="2"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A2" s="11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B2" s="11" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D2" s="11"/>
       <c r="E2" s="11" t="s">
@@ -978,7 +981,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A3" s="11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B3" s="11" t="s">
         <v>4</v>
@@ -998,7 +1001,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A4" s="16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B4" s="16"/>
       <c r="C4" s="16" t="s">
@@ -1011,12 +1014,12 @@
       <c r="F4" s="16"/>
       <c r="G4" s="16"/>
       <c r="H4" s="24" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A5" s="11" t="s">
-        <v>5</v>
+        <v>101</v>
       </c>
       <c r="B5" s="11" t="s">
         <v>4</v>
@@ -1034,7 +1037,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A6" s="11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B6" s="11" t="s">
         <v>4</v>
@@ -1052,7 +1055,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>4</v>
@@ -1067,12 +1070,12 @@
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
       <c r="H7" s="25" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>4</v>
@@ -1087,12 +1090,12 @@
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
       <c r="H8" s="26" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A9" s="11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B9" s="11" t="s">
         <v>4</v>
@@ -1112,7 +1115,7 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A10" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B10" s="7" t="s">
         <v>4</v>
@@ -1127,30 +1130,30 @@
       <c r="F10" s="7"/>
       <c r="G10" s="7"/>
       <c r="H10" s="18" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" hidden="1" x14ac:dyDescent="0.15">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A11" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="B11" s="12" t="s">
         <v>77</v>
-      </c>
-      <c r="B11" s="12" t="s">
-        <v>78</v>
       </c>
       <c r="C11" s="12"/>
       <c r="D11" s="12" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E11" s="12"/>
       <c r="F11" s="12"/>
       <c r="G11" s="12"/>
       <c r="H11" s="19" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A12" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B12" s="7"/>
       <c r="C12" s="7" t="s">
@@ -1162,13 +1165,13 @@
       </c>
       <c r="F12" s="7"/>
       <c r="G12" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H12" s="8"/>
     </row>
-    <row r="13" spans="1:9" hidden="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A13" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B13" s="7" t="s">
         <v>4</v>
@@ -1181,12 +1184,12 @@
       <c r="F13" s="7"/>
       <c r="G13" s="7"/>
       <c r="H13" s="18" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A14" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B14" s="7" t="s">
         <v>4</v>
@@ -1201,7 +1204,7 @@
       <c r="F14" s="7"/>
       <c r="G14" s="7"/>
       <c r="H14" s="18" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.15">
@@ -1226,7 +1229,7 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A16" s="11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B16" s="11" t="s">
         <v>4</v>
@@ -1244,9 +1247,9 @@
       <c r="G16" s="11"/>
       <c r="H16" s="12"/>
     </row>
-    <row r="17" spans="1:8" hidden="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A17" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>4</v>
@@ -1259,12 +1262,12 @@
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
       <c r="H17" s="26" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A18" s="11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B18" s="11" t="s">
         <v>4</v>
@@ -1282,7 +1285,7 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A19" s="11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B19" s="11"/>
       <c r="C19" s="11" t="s">
@@ -1295,12 +1298,12 @@
       <c r="F19" s="11"/>
       <c r="G19" s="11"/>
       <c r="H19" s="19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A20" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B20" s="5"/>
       <c r="C20" s="5" t="s">
@@ -1315,12 +1318,12 @@
         <v>4</v>
       </c>
       <c r="H20" s="20" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A21" s="11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B21" s="11" t="s">
         <v>4</v>
@@ -1340,7 +1343,7 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A22" s="11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B22" s="11" t="s">
         <v>4</v>
@@ -1356,9 +1359,9 @@
       <c r="G22" s="11"/>
       <c r="H22" s="12"/>
     </row>
-    <row r="23" spans="1:8" hidden="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A23" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>4</v>
@@ -1371,216 +1374,212 @@
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
       <c r="H23" s="21" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A24" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="B24" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C24" s="11"/>
+      <c r="D24" s="11"/>
+      <c r="E24" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="F24" s="11"/>
+      <c r="G24" s="11"/>
+      <c r="H24" s="12"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A25" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="B25" s="16"/>
+      <c r="C25" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="D25" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="E25" s="16"/>
+      <c r="F25" s="16"/>
+      <c r="G25" s="16"/>
+      <c r="H25" s="24" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A26" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B26" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="C26" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D26" s="13"/>
+      <c r="E26" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="F26" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="G26" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="H26" s="14"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A27" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="B27" s="11"/>
+      <c r="C27" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D27" s="11"/>
+      <c r="E27" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="F27" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="G27" s="11"/>
+      <c r="H27" s="12"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A28" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="B28" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="C28" s="16"/>
+      <c r="D28" s="16"/>
+      <c r="E28" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="F28" s="16"/>
+      <c r="G28" s="16"/>
+      <c r="H28" s="17"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A29" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="B29" s="11"/>
+      <c r="C29" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D29" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="E29" s="11"/>
+      <c r="F29" s="11"/>
+      <c r="G29" s="11"/>
+      <c r="H29" s="19" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A30" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="B30" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="C30" s="14"/>
+      <c r="D30" s="14"/>
+      <c r="E30" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="F30" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="G30" s="13"/>
+      <c r="H30" s="14"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A31" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="B31" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="C31" s="12"/>
+      <c r="D31" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="E31" s="12"/>
+      <c r="F31" s="12"/>
+      <c r="G31" s="12"/>
+      <c r="H31" s="19" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A32" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B32" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C32" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D32" s="9"/>
+      <c r="E32" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="F32" s="9"/>
+      <c r="G32" s="9"/>
+      <c r="H32" s="10"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A33" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="B33" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="C33" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="D33" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="E33" s="15"/>
+      <c r="F33" s="15"/>
+      <c r="G33" s="15"/>
+      <c r="H33" s="22" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A24" s="16" t="s">
-        <v>76</v>
-      </c>
-      <c r="B24" s="16"/>
-      <c r="C24" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="D24" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="E24" s="16"/>
-      <c r="F24" s="16"/>
-      <c r="G24" s="16"/>
-      <c r="H24" s="24" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A25" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="B25" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="C25" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="D25" s="13"/>
-      <c r="E25" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="F25" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="G25" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="H25" s="14"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A26" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="B26" s="11"/>
-      <c r="C26" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="D26" s="11"/>
-      <c r="E26" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="F26" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="G26" s="11"/>
-      <c r="H26" s="12"/>
-    </row>
-    <row r="27" spans="1:8" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A27" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="B27" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="C27" s="16"/>
-      <c r="D27" s="16"/>
-      <c r="E27" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="F27" s="16"/>
-      <c r="G27" s="16"/>
-      <c r="H27" s="17"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A28" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="B28" s="11"/>
-      <c r="C28" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="D28" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="E28" s="11"/>
-      <c r="F28" s="11"/>
-      <c r="G28" s="11"/>
-      <c r="H28" s="19" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A29" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="B29" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="C29" s="14"/>
-      <c r="D29" s="14"/>
-      <c r="E29" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="F29" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="G29" s="13"/>
-      <c r="H29" s="14"/>
-    </row>
-    <row r="30" spans="1:8" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A30" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="B30" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="C30" s="12"/>
-      <c r="D30" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="E30" s="12"/>
-      <c r="F30" s="12"/>
-      <c r="G30" s="12"/>
-      <c r="H30" s="19" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A31" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B31" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="C31" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D31" s="9"/>
-      <c r="E31" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="F31" s="9"/>
-      <c r="G31" s="9"/>
-      <c r="H31" s="10"/>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A32" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="B32" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="C32" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="D32" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="E32" s="15"/>
-      <c r="F32" s="15"/>
-      <c r="G32" s="15"/>
-      <c r="H32" s="22" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A33" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B33" s="3"/>
-      <c r="C33" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D33" s="3"/>
-      <c r="E33" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F33" s="3"/>
-      <c r="G33" s="3"/>
-      <c r="H33" s="4"/>
-    </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A34" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="B34" s="11"/>
-      <c r="C34" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="D34" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="E34" s="11"/>
-      <c r="F34" s="11"/>
-      <c r="G34" s="11"/>
-      <c r="H34" s="19" t="s">
-        <v>62</v>
-      </c>
+      <c r="A34" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B34" s="3"/>
+      <c r="C34" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D34" s="3"/>
+      <c r="E34" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F34" s="3"/>
+      <c r="G34" s="3"/>
+      <c r="H34" s="4"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A35" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="B35" s="11" t="s">
-        <v>4</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="B35" s="11"/>
       <c r="C35" s="11" t="s">
         <v>4</v>
       </c>
@@ -1591,12 +1590,12 @@
       <c r="F35" s="11"/>
       <c r="G35" s="11"/>
       <c r="H35" s="19" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A36" s="11" t="s">
-        <v>47</v>
+        <v>19</v>
       </c>
       <c r="B36" s="11" t="s">
         <v>4</v>
@@ -1604,95 +1603,93 @@
       <c r="C36" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D36" s="11"/>
-      <c r="E36" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="F36" s="11" t="s">
-        <v>4</v>
-      </c>
+      <c r="D36" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="E36" s="11"/>
+      <c r="F36" s="11"/>
       <c r="G36" s="11"/>
-      <c r="H36" s="12"/>
+      <c r="H36" s="19" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A37" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B37" s="3"/>
-      <c r="C37" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D37" s="3"/>
-      <c r="E37" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F37" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="G37" s="3"/>
-      <c r="H37" s="4"/>
+      <c r="A37" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="B37" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C37" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D37" s="11"/>
+      <c r="E37" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="F37" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="G37" s="11"/>
+      <c r="H37" s="12"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A38" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B38" s="3"/>
       <c r="C38" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D38" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E38" s="3"/>
-      <c r="F38" s="3"/>
+      <c r="D38" s="3"/>
+      <c r="E38" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F38" s="3" t="s">
+        <v>4</v>
+      </c>
       <c r="G38" s="3"/>
-      <c r="H38" s="26" t="s">
+      <c r="H38" s="4"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A39" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B39" s="3"/>
+      <c r="C39" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E39" s="3"/>
+      <c r="F39" s="3"/>
+      <c r="G39" s="3"/>
+      <c r="H39" s="26" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A40" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="B40" s="11"/>
+      <c r="C40" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D40" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="E40" s="11"/>
+      <c r="F40" s="11"/>
+      <c r="G40" s="11"/>
+      <c r="H40" s="19" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A39" s="11" t="s">
-        <v>99</v>
-      </c>
-      <c r="B39" s="11"/>
-      <c r="C39" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="D39" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="E39" s="11"/>
-      <c r="F39" s="11"/>
-      <c r="G39" s="11"/>
-      <c r="H39" s="19" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A40" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="B40" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="C40" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="D40" s="13"/>
-      <c r="E40" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="F40" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="G40" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="H40" s="14"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A41" s="13" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B41" s="13" t="s">
         <v>4</v>
@@ -1708,49 +1705,51 @@
         <v>4</v>
       </c>
       <c r="G41" s="13" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H41" s="14"/>
     </row>
-    <row r="42" spans="1:8" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A42" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="B42" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="C42" s="11"/>
-      <c r="D42" s="11"/>
-      <c r="E42" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="F42" s="11"/>
-      <c r="G42" s="11"/>
-      <c r="H42" s="12"/>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A42" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B42" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="C42" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D42" s="13"/>
+      <c r="E42" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="F42" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="G42" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="H42" s="14"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A43" s="11" t="s">
-        <v>90</v>
+        <v>30</v>
       </c>
       <c r="B43" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C43" s="11" t="s">
-        <v>4</v>
-      </c>
+      <c r="C43" s="11"/>
       <c r="D43" s="11"/>
       <c r="E43" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="F43" s="11" t="s">
-        <v>4</v>
-      </c>
+      <c r="F43" s="11"/>
       <c r="G43" s="11"/>
       <c r="H43" s="12"/>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A44" s="11" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B44" s="11" t="s">
         <v>4</v>
@@ -1769,104 +1768,104 @@
       <c r="H44" s="12"/>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A45" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B45" s="3"/>
-      <c r="C45" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D45" s="3"/>
-      <c r="E45" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F45" s="3"/>
-      <c r="G45" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="H45" s="4"/>
+      <c r="A45" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="B45" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C45" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D45" s="11"/>
+      <c r="E45" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="F45" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="G45" s="11"/>
+      <c r="H45" s="12"/>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A46" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B46" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="C46" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D46" s="9"/>
-      <c r="E46" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="F46" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="G46" s="9"/>
-      <c r="H46" s="10"/>
-    </row>
-    <row r="47" spans="1:8" hidden="1" x14ac:dyDescent="0.15">
+      <c r="A46" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B46" s="3"/>
+      <c r="C46" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D46" s="3"/>
+      <c r="E46" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F46" s="3"/>
+      <c r="G46" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="H46" s="4"/>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A47" s="9" t="s">
-        <v>37</v>
+        <v>13</v>
       </c>
       <c r="B47" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C47" s="9"/>
-      <c r="D47" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="E47" s="9"/>
-      <c r="F47" s="9"/>
+      <c r="C47" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D47" s="9"/>
+      <c r="E47" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="F47" s="9" t="s">
+        <v>4</v>
+      </c>
       <c r="G47" s="9"/>
-      <c r="H47" s="23" t="s">
-        <v>71</v>
-      </c>
+      <c r="H47" s="10"/>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A48" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B48" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C48" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D48" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="E48" s="5"/>
-      <c r="F48" s="5"/>
-      <c r="G48" s="5"/>
-      <c r="H48" s="20" t="s">
-        <v>73</v>
+      <c r="A48" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B48" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C48" s="9"/>
+      <c r="D48" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E48" s="9"/>
+      <c r="F48" s="9"/>
+      <c r="G48" s="9"/>
+      <c r="H48" s="23" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A49" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="B49" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="C49" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="D49" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="E49" s="11"/>
-      <c r="F49" s="11"/>
-      <c r="G49" s="11"/>
-      <c r="H49" s="19" t="s">
-        <v>69</v>
+      <c r="A49" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B49" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C49" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D49" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E49" s="5"/>
+      <c r="F49" s="5"/>
+      <c r="G49" s="5"/>
+      <c r="H49" s="20" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A50" s="11" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B50" s="11" t="s">
         <v>4</v>
@@ -1874,19 +1873,19 @@
       <c r="C50" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D50" s="11"/>
-      <c r="E50" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="F50" s="11" t="s">
-        <v>4</v>
-      </c>
+      <c r="D50" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="E50" s="11"/>
+      <c r="F50" s="11"/>
       <c r="G50" s="11"/>
-      <c r="H50" s="12"/>
+      <c r="H50" s="19" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A51" s="11" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B51" s="11" t="s">
         <v>4</v>
@@ -1904,14 +1903,16 @@
       <c r="G51" s="11"/>
       <c r="H51" s="12"/>
     </row>
-    <row r="52" spans="1:8" hidden="1" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A52" s="11" t="s">
-        <v>95</v>
+        <v>18</v>
       </c>
       <c r="B52" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C52" s="11"/>
+      <c r="C52" s="11" t="s">
+        <v>4</v>
+      </c>
       <c r="D52" s="11"/>
       <c r="E52" s="11" t="s">
         <v>4</v>
@@ -1922,7 +1923,7 @@
       <c r="G52" s="11"/>
       <c r="H52" s="12"/>
     </row>
-    <row r="53" spans="1:8" hidden="1" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A53" s="11" t="s">
         <v>94</v>
       </c>
@@ -1930,175 +1931,188 @@
         <v>4</v>
       </c>
       <c r="C53" s="11"/>
-      <c r="D53" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="E53" s="11"/>
-      <c r="F53" s="11"/>
+      <c r="D53" s="11"/>
+      <c r="E53" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="F53" s="11" t="s">
+        <v>4</v>
+      </c>
       <c r="G53" s="11"/>
-      <c r="H53" s="19" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" hidden="1" x14ac:dyDescent="0.15">
+      <c r="H53" s="12"/>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A54" s="11" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B54" s="11" t="s">
-        <v>79</v>
+        <v>4</v>
       </c>
       <c r="C54" s="11"/>
-      <c r="D54" s="11"/>
-      <c r="E54" s="11" t="s">
-        <v>4</v>
-      </c>
+      <c r="D54" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="E54" s="11"/>
       <c r="F54" s="11"/>
       <c r="G54" s="11"/>
-      <c r="H54" s="19"/>
+      <c r="H54" s="19" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A55" s="11" t="s">
-        <v>12</v>
+        <v>97</v>
       </c>
       <c r="B55" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="C55" s="11" t="s">
-        <v>4</v>
-      </c>
+        <v>78</v>
+      </c>
+      <c r="C55" s="11"/>
       <c r="D55" s="11"/>
       <c r="E55" s="11" t="s">
         <v>4</v>
       </c>
       <c r="F55" s="11"/>
       <c r="G55" s="11"/>
-      <c r="H55" s="12"/>
-    </row>
-    <row r="56" spans="1:8" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A56" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="B56" s="10" t="s">
-        <v>78</v>
-      </c>
-      <c r="C56" s="10"/>
-      <c r="D56" s="10" t="s">
-        <v>78</v>
-      </c>
-      <c r="E56" s="10"/>
-      <c r="F56" s="10"/>
-      <c r="G56" s="10"/>
-      <c r="H56" s="23" t="s">
-        <v>84</v>
-      </c>
+      <c r="H55" s="19"/>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A56" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B56" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C56" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D56" s="11"/>
+      <c r="E56" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="F56" s="11"/>
+      <c r="G56" s="11"/>
+      <c r="H56" s="12"/>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A57" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B57" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="C57" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D57" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="E57" s="9"/>
-      <c r="F57" s="9"/>
-      <c r="G57" s="9"/>
+        <v>81</v>
+      </c>
+      <c r="B57" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="C57" s="10"/>
+      <c r="D57" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="E57" s="10"/>
+      <c r="F57" s="10"/>
+      <c r="G57" s="10"/>
       <c r="H57" s="23" t="s">
-        <v>74</v>
+        <v>83</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A58" s="11" t="s">
-        <v>83</v>
-      </c>
-      <c r="B58" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="C58" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="D58" s="11"/>
-      <c r="E58" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="F58" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="G58" s="11"/>
-      <c r="H58" s="12"/>
+      <c r="A58" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B58" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C58" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D58" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E58" s="9"/>
+      <c r="F58" s="9"/>
+      <c r="G58" s="9"/>
+      <c r="H58" s="23" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A59" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="B59" s="11"/>
+        <v>82</v>
+      </c>
+      <c r="B59" s="11" t="s">
+        <v>4</v>
+      </c>
       <c r="C59" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D59" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="E59" s="11"/>
-      <c r="F59" s="11"/>
+      <c r="D59" s="11"/>
+      <c r="E59" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="F59" s="11" t="s">
+        <v>4</v>
+      </c>
       <c r="G59" s="11"/>
-      <c r="H59" s="19" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A60" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="B60" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="C60" s="15"/>
-      <c r="D60" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="E60" s="15"/>
-      <c r="F60" s="15"/>
-      <c r="G60" s="15"/>
-      <c r="H60" s="22" t="s">
-        <v>72</v>
+      <c r="H59" s="12"/>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A60" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B60" s="11"/>
+      <c r="C60" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D60" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="E60" s="11"/>
+      <c r="F60" s="11"/>
+      <c r="G60" s="11"/>
+      <c r="H60" s="19" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A61" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="B61" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="C61" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="D61" s="13"/>
-      <c r="E61" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="F61" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="G61" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="H61" s="14"/>
+      <c r="A61" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="B61" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="C61" s="15"/>
+      <c r="D61" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="E61" s="15"/>
+      <c r="F61" s="15"/>
+      <c r="G61" s="15"/>
+      <c r="H61" s="22" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A62" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="B62" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="C62" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D62" s="13"/>
+      <c r="E62" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="F62" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="G62" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="H62" s="14"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H61">
-    <filterColumn colId="2">
-      <customFilters>
-        <customFilter operator="notEqual" val=" "/>
-      </customFilters>
-    </filterColumn>
-    <sortState ref="A2:G61">
-      <sortCondition ref="A1:A60"/>
+  <autoFilter ref="A1:H62">
+    <sortState ref="A2:H62">
+      <sortCondition ref="A1:A62"/>
     </sortState>
   </autoFilter>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -2116,25 +2130,25 @@
     <hyperlink ref="H14" r:id="rId6"/>
     <hyperlink ref="H17" r:id="rId7"/>
     <hyperlink ref="H19" r:id="rId8"/>
-    <hyperlink ref="H34" r:id="rId9"/>
+    <hyperlink ref="H35" r:id="rId9"/>
     <hyperlink ref="H20" r:id="rId10"/>
     <hyperlink ref="H23" r:id="rId11"/>
-    <hyperlink ref="H32" r:id="rId12"/>
-    <hyperlink ref="H35" r:id="rId13"/>
-    <hyperlink ref="H38" r:id="rId14"/>
-    <hyperlink ref="H39" r:id="rId15"/>
-    <hyperlink ref="H49" r:id="rId16"/>
-    <hyperlink ref="H59" r:id="rId17"/>
-    <hyperlink ref="H47" r:id="rId18" location="/download"/>
-    <hyperlink ref="H60" r:id="rId19"/>
-    <hyperlink ref="H48" r:id="rId20"/>
-    <hyperlink ref="H57" r:id="rId21"/>
-    <hyperlink ref="H24" r:id="rId22"/>
+    <hyperlink ref="H33" r:id="rId12"/>
+    <hyperlink ref="H36" r:id="rId13"/>
+    <hyperlink ref="H39" r:id="rId14"/>
+    <hyperlink ref="H40" r:id="rId15"/>
+    <hyperlink ref="H50" r:id="rId16"/>
+    <hyperlink ref="H60" r:id="rId17"/>
+    <hyperlink ref="H48" r:id="rId18" location="/download"/>
+    <hyperlink ref="H61" r:id="rId19"/>
+    <hyperlink ref="H49" r:id="rId20"/>
+    <hyperlink ref="H58" r:id="rId21"/>
+    <hyperlink ref="H25" r:id="rId22"/>
     <hyperlink ref="H11" r:id="rId23"/>
-    <hyperlink ref="H56" r:id="rId24" location="Windows"/>
-    <hyperlink ref="H30" r:id="rId25"/>
-    <hyperlink ref="H28" r:id="rId26"/>
-    <hyperlink ref="H53" r:id="rId27"/>
+    <hyperlink ref="H57" r:id="rId24" location="Windows"/>
+    <hyperlink ref="H31" r:id="rId25"/>
+    <hyperlink ref="H29" r:id="rId26"/>
+    <hyperlink ref="H54" r:id="rId27"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId28"/>

</xml_diff>

<commit_message>
Update on 20220110 part 2
</commit_message>
<xml_diff>
--- a/文档/其他文档/Others/PC/一体机和笔记本软件列表.xlsx
+++ b/文档/其他文档/Others/PC/一体机和笔记本软件列表.xlsx
@@ -12,14 +12,14 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$H$69</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$H$70</definedName>
   </definedNames>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="112">
   <si>
     <t>是否绿色版</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -461,6 +461,10 @@
   </si>
   <si>
     <t>LanDrop（局域网内文件传输工具）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>下载工具 BitComet比特彗星 (隐藏功能解锁版)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -630,14 +634,7 @@
     <cellStyle name="常规" xfId="0" builtinId="0"/>
     <cellStyle name="超链接" xfId="1" builtinId="8"/>
   </cellStyles>
-  <dxfs count="5">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="4">
     <dxf>
       <fill>
         <patternFill>
@@ -974,13 +971,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I69"/>
+  <dimension ref="A1:I70"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="42.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="45.125" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="13.875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20.5" bestFit="1" customWidth="1"/>
@@ -2018,7 +2015,7 @@
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A55" s="9" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="B55" s="9" t="s">
         <v>4</v>
@@ -2038,7 +2035,7 @@
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A56" s="9" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B56" s="9" t="s">
         <v>4</v>
@@ -2058,7 +2055,7 @@
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A57" s="9" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B57" s="9" t="s">
         <v>4</v>
@@ -2078,7 +2075,7 @@
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A58" s="9" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B58" s="9" t="s">
         <v>4</v>
@@ -2094,11 +2091,11 @@
         <v>4</v>
       </c>
       <c r="G58" s="9"/>
-      <c r="H58" s="10"/>
+      <c r="H58" s="16"/>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A59" s="9" t="s">
-        <v>17</v>
+        <v>104</v>
       </c>
       <c r="B59" s="9" t="s">
         <v>4</v>
@@ -2118,12 +2115,14 @@
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A60" s="9" t="s">
-        <v>85</v>
+        <v>17</v>
       </c>
       <c r="B60" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C60" s="9"/>
+      <c r="C60" s="9" t="s">
+        <v>4</v>
+      </c>
       <c r="D60" s="9"/>
       <c r="E60" s="9" t="s">
         <v>4</v>
@@ -2136,194 +2135,212 @@
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A61" s="9" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B61" s="9" t="s">
         <v>4</v>
       </c>
       <c r="C61" s="9"/>
-      <c r="D61" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="E61" s="9"/>
-      <c r="F61" s="9"/>
+      <c r="D61" s="9"/>
+      <c r="E61" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="F61" s="9" t="s">
+        <v>4</v>
+      </c>
       <c r="G61" s="9"/>
-      <c r="H61" s="16" t="s">
-        <v>86</v>
-      </c>
+      <c r="H61" s="10"/>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A62" s="9" t="s">
-        <v>105</v>
+        <v>84</v>
       </c>
       <c r="B62" s="9" t="s">
-        <v>73</v>
+        <v>4</v>
       </c>
       <c r="C62" s="9"/>
-      <c r="D62" s="9"/>
-      <c r="E62" s="9" t="s">
-        <v>4</v>
-      </c>
+      <c r="D62" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E62" s="9"/>
       <c r="F62" s="9"/>
       <c r="G62" s="9"/>
-      <c r="H62" s="16"/>
+      <c r="H62" s="16" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A63" s="9" t="s">
-        <v>10</v>
+        <v>105</v>
       </c>
       <c r="B63" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="C63" s="9" t="s">
-        <v>4</v>
-      </c>
+        <v>73</v>
+      </c>
+      <c r="C63" s="9"/>
       <c r="D63" s="9"/>
       <c r="E63" s="9" t="s">
         <v>4</v>
       </c>
       <c r="F63" s="9"/>
       <c r="G63" s="9"/>
-      <c r="H63" s="10"/>
+      <c r="H63" s="16"/>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A64" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="B64" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="C64" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="D64" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="E64" s="8"/>
-      <c r="F64" s="8"/>
-      <c r="G64" s="8"/>
-      <c r="H64" s="19" t="s">
-        <v>77</v>
-      </c>
+      <c r="A64" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B64" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C64" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D64" s="9"/>
+      <c r="E64" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="F64" s="9"/>
+      <c r="G64" s="9"/>
+      <c r="H64" s="10"/>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A65" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="B65" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="C65" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D65" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="E65" s="8"/>
+      <c r="F65" s="8"/>
+      <c r="G65" s="8"/>
+      <c r="H65" s="19" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A66" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B65" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C65" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="D65" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="E65" s="7"/>
-      <c r="F65" s="7"/>
-      <c r="G65" s="7"/>
-      <c r="H65" s="19" t="s">
+      <c r="B66" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C66" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D66" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E66" s="7"/>
+      <c r="F66" s="7"/>
+      <c r="G66" s="7"/>
+      <c r="H66" s="19" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A66" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="B66" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="C66" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D66" s="9"/>
-      <c r="E66" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="F66" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="G66" s="9"/>
-      <c r="H66" s="10"/>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A67" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="B67" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C67" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D67" s="9"/>
+      <c r="E67" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="F67" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="G67" s="9"/>
+      <c r="H67" s="10"/>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A68" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="B67" s="9"/>
-      <c r="C67" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D67" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="E67" s="9"/>
-      <c r="F67" s="9"/>
-      <c r="G67" s="9"/>
-      <c r="H67" s="16" t="s">
+      <c r="B68" s="9"/>
+      <c r="C68" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D68" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E68" s="9"/>
+      <c r="F68" s="9"/>
+      <c r="G68" s="9"/>
+      <c r="H68" s="16" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A68" s="13" t="s">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A69" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="B68" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="C68" s="13"/>
-      <c r="D68" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="E68" s="13"/>
-      <c r="F68" s="13"/>
-      <c r="G68" s="13"/>
-      <c r="H68" s="18" t="s">
+      <c r="B69" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="C69" s="13"/>
+      <c r="D69" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="E69" s="13"/>
+      <c r="F69" s="13"/>
+      <c r="G69" s="13"/>
+      <c r="H69" s="18" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A69" s="11" t="s">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A70" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="B69" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="C69" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="D69" s="11"/>
-      <c r="E69" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="F69" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="G69" s="11" t="s">
+      <c r="B70" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C70" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D70" s="11"/>
+      <c r="E70" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="F70" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="G70" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="H69" s="12"/>
+      <c r="H70" s="12"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H69">
-    <sortState ref="A2:H69">
-      <sortCondition ref="A1:A69"/>
+  <autoFilter ref="A1:H70">
+    <sortState ref="A2:H70">
+      <sortCondition ref="A1:A70"/>
     </sortState>
   </autoFilter>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="A1:A57 A60:A1048576">
+  <conditionalFormatting sqref="A61:A1048576 A1:A58">
     <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="浏览器">
       <formula>NOT(ISERROR(SEARCH("浏览器",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A58">
+  <conditionalFormatting sqref="A59">
     <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="浏览器">
-      <formula>NOT(ISERROR(SEARCH("浏览器",A58)))</formula>
+      <formula>NOT(ISERROR(SEARCH("浏览器",A59)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A59">
+  <conditionalFormatting sqref="A60">
     <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="浏览器">
-      <formula>NOT(ISERROR(SEARCH("浏览器",A59)))</formula>
+      <formula>NOT(ISERROR(SEARCH("浏览器",A60)))</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
@@ -2341,17 +2358,17 @@
     <hyperlink ref="H42" r:id="rId12"/>
     <hyperlink ref="H43" r:id="rId13"/>
     <hyperlink ref="H53" r:id="rId14"/>
-    <hyperlink ref="H67" r:id="rId15"/>
+    <hyperlink ref="H68" r:id="rId15"/>
     <hyperlink ref="H51" r:id="rId16" location="/download"/>
-    <hyperlink ref="H68" r:id="rId17"/>
+    <hyperlink ref="H69" r:id="rId17"/>
     <hyperlink ref="H52" r:id="rId18"/>
-    <hyperlink ref="H65" r:id="rId19"/>
+    <hyperlink ref="H66" r:id="rId19"/>
     <hyperlink ref="H28" r:id="rId20"/>
     <hyperlink ref="H12" r:id="rId21"/>
-    <hyperlink ref="H64" r:id="rId22" location="Windows"/>
+    <hyperlink ref="H65" r:id="rId22" location="Windows"/>
     <hyperlink ref="H36" r:id="rId23"/>
     <hyperlink ref="H32" r:id="rId24"/>
-    <hyperlink ref="H61" r:id="rId25"/>
+    <hyperlink ref="H62" r:id="rId25"/>
     <hyperlink ref="H18" r:id="rId26"/>
     <hyperlink ref="H19" r:id="rId27"/>
   </hyperlinks>

</xml_diff>

<commit_message>
Update on 20220207 part 2
</commit_message>
<xml_diff>
--- a/文档/其他文档/Others/PC/一体机和笔记本软件列表.xlsx
+++ b/文档/其他文档/Others/PC/一体机和笔记本软件列表.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="109">
   <si>
     <t>是否绿色版</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -453,10 +453,6 @@
   </si>
   <si>
     <t>https://potplayer.daum.net/</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://www.internetdownloadmanager.com/</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1987,15 +1983,15 @@
       <c r="C53" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="D53" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="E53" s="9"/>
-      <c r="F53" s="9"/>
+      <c r="D53" s="9"/>
+      <c r="E53" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="F53" s="9" t="s">
+        <v>4</v>
+      </c>
       <c r="G53" s="9"/>
-      <c r="H53" s="16" t="s">
-        <v>109</v>
-      </c>
+      <c r="H53" s="16"/>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A54" s="9" t="s">
@@ -2320,10 +2316,9 @@
     <hyperlink ref="H59" r:id="rId25"/>
     <hyperlink ref="H18" r:id="rId26"/>
     <hyperlink ref="H54" r:id="rId27"/>
-    <hyperlink ref="H53" r:id="rId28"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId29"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId28"/>
 </worksheet>
 </file>
 

</xml_diff>